<commit_message>
fix template data aktor
</commit_message>
<xml_diff>
--- a/analisa/data aktor.xlsx
+++ b/analisa/data aktor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\SIAKES\analisa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A529D4F6-39B7-4281-A790-CB2DAD68B59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4751A5-C416-449A-9EC3-76467A021374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>tb_siswa</t>
   </si>
@@ -51,21 +51,12 @@
     <t>nama</t>
   </si>
   <si>
-    <t>tpl</t>
-  </si>
-  <si>
-    <t>tgl</t>
-  </si>
-  <si>
     <t>jk</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>hp</t>
-  </si>
-  <si>
     <t>id_kelas</t>
   </si>
   <si>
@@ -117,21 +108,12 @@
     <t>ANANG MAULANA</t>
   </si>
   <si>
-    <t>Laki-Laki</t>
-  </si>
-  <si>
     <t>ASEP TAMAMI</t>
   </si>
   <si>
     <t>Subang</t>
   </si>
   <si>
-    <t>02 Januari 2009</t>
-  </si>
-  <si>
-    <t>05 April 2009</t>
-  </si>
-  <si>
     <t>083833679726</t>
   </si>
   <si>
@@ -162,12 +144,6 @@
     <t>HAIKAL</t>
   </si>
   <si>
-    <t>27 Juni 2009</t>
-  </si>
-  <si>
-    <t>25 Agustus 2008</t>
-  </si>
-  <si>
     <t>anjasmalisi@gmail.com</t>
   </si>
   <si>
@@ -192,15 +168,6 @@
     <t>JIHAN</t>
   </si>
   <si>
-    <t>31 Juli 2008</t>
-  </si>
-  <si>
-    <t>01 Januari 2008</t>
-  </si>
-  <si>
-    <t>Perempuan</t>
-  </si>
-  <si>
     <t>friyfauziah@gmail.com</t>
   </si>
   <si>
@@ -225,9 +192,6 @@
     <t>SAEPUL JAMIL</t>
   </si>
   <si>
-    <t>04 Juni 2007</t>
-  </si>
-  <si>
     <t>rikis0325@gmail.com</t>
   </si>
   <si>
@@ -282,24 +246,6 @@
     <t>Ciamis</t>
   </si>
   <si>
-    <t>25 September 2007</t>
-  </si>
-  <si>
-    <t>04 Oktober 2006</t>
-  </si>
-  <si>
-    <t>09 Agustus 2006</t>
-  </si>
-  <si>
-    <t>14 Mei 2006</t>
-  </si>
-  <si>
-    <t>14 Maret 2007</t>
-  </si>
-  <si>
-    <t>22 Januari 2007</t>
-  </si>
-  <si>
     <t>085176866872</t>
   </si>
   <si>
@@ -354,9 +300,6 @@
     <t>Kota Baru</t>
   </si>
   <si>
-    <t>18 Maret 1994</t>
-  </si>
-  <si>
     <t>081382541384</t>
   </si>
   <si>
@@ -369,12 +312,6 @@
     <t>081394440445</t>
   </si>
   <si>
-    <t>27 September 1989</t>
-  </si>
-  <si>
-    <t>27 September 1993</t>
-  </si>
-  <si>
     <t>1602022705990002</t>
   </si>
   <si>
@@ -390,9 +327,6 @@
     <t>Tanjung Baru</t>
   </si>
   <si>
-    <t>25 Mei 1999</t>
-  </si>
-  <si>
     <t>muksinadithya@gmail.com</t>
   </si>
   <si>
@@ -400,13 +334,31 @@
   </si>
   <si>
     <t>atinrohaeni93@gmail.com</t>
+  </si>
+  <si>
+    <t>tempat_lahir</t>
+  </si>
+  <si>
+    <t>tanggal_lahir</t>
+  </si>
+  <si>
+    <t>no_hp</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,8 +406,38 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,8 +450,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FF5B9BD5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -568,12 +556,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -602,9 +627,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,9 +636,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -665,12 +684,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -695,14 +708,70 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -987,79 +1056,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="33"/>
-    <col min="2" max="2" width="19.33203125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" style="35" customWidth="1"/>
-    <col min="4" max="4" width="14" style="35" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="36" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" style="37" customWidth="1"/>
-    <col min="9" max="16" width="9.109375" style="33"/>
-    <col min="17" max="17" width="12.44140625" style="33" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" style="33" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="33"/>
+    <col min="1" max="1" width="9.109375" style="29"/>
+    <col min="2" max="2" width="19.33203125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" style="31" customWidth="1"/>
+    <col min="4" max="4" width="14" style="31" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="32" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="33" customWidth="1"/>
+    <col min="9" max="16" width="9.109375" style="29"/>
+    <col min="17" max="17" width="12.44140625" style="29" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="29" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="P1" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="43"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="P1" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="39"/>
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="K2" s="46" t="s">
         <v>8</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>1</v>
@@ -1068,41 +1137,41 @@
         <v>3</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="48">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="8">
+      <c r="B3" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="50">
+        <v>39991</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="54">
         <v>1</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="54">
         <v>7</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="54">
         <v>4</v>
       </c>
       <c r="P3" s="6">
@@ -1112,41 +1181,41 @@
         <v>10</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="48">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="50">
+        <v>39685</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="8">
+      <c r="H4" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="54">
         <v>1</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="54">
         <v>7</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="54">
         <v>4</v>
       </c>
       <c r="P4" s="6">
@@ -1156,41 +1225,41 @@
         <v>11</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="48">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="50">
+        <v>39908</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="8">
+      <c r="I5" s="54">
         <v>1</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="54">
         <v>8</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="54">
         <v>4</v>
       </c>
       <c r="P5" s="8">
@@ -1200,640 +1269,640 @@
         <v>12</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="48">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="50">
+        <v>39815</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="H6" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="8">
+      <c r="I6" s="54">
         <v>1</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="54">
         <v>8</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="54">
         <v>4</v>
       </c>
       <c r="P6" s="8">
         <v>4</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="48">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" s="8">
+      <c r="B7" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="50">
+        <v>39237</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="54">
         <v>2</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="54">
         <v>7</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="54">
         <v>5</v>
       </c>
       <c r="P7" s="8">
         <v>5</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="48">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="B8" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="50">
+        <v>39448</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="8">
+      <c r="H8" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="54">
         <v>2</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="54">
         <v>7</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="54">
         <v>5</v>
       </c>
       <c r="P8" s="8">
         <v>6</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="48">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="8">
+      <c r="B9" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="50">
+        <v>39660</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="54">
         <v>2</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="54">
         <v>8</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="54">
         <v>5</v>
       </c>
       <c r="P9" s="8">
         <v>7</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+      <c r="A10" s="48">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="8">
+      <c r="B10" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="50">
+        <v>39448</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="54">
         <v>2</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="54">
         <v>8</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="54">
         <v>5</v>
       </c>
       <c r="P10" s="8">
         <v>8</v>
       </c>
       <c r="Q10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="48">
+        <v>9</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="R10" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="8">
+      <c r="E11" s="50">
+        <v>39350</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="54">
         <v>3</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="54">
         <v>7</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="54">
         <v>6</v>
       </c>
       <c r="P11" s="8">
         <v>9</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="48">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="50">
+        <v>38994</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="54">
+        <v>3</v>
+      </c>
+      <c r="J12" s="54">
+        <v>7</v>
+      </c>
+      <c r="K12" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="48">
+        <v>11</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="E13" s="50">
+        <v>38938</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="54">
+        <v>3</v>
+      </c>
+      <c r="J13" s="54">
+        <v>8</v>
+      </c>
+      <c r="K13" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="48">
+        <v>12</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="50">
+        <v>38851</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="54">
+        <v>3</v>
+      </c>
+      <c r="J14" s="54">
+        <v>8</v>
+      </c>
+      <c r="K14" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="48">
+        <v>13</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="50">
+        <v>39155</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="54">
+        <v>3</v>
+      </c>
+      <c r="J15" s="54">
+        <v>9</v>
+      </c>
+      <c r="K15" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="48">
+        <v>14</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="50">
+        <v>39104</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="8">
+      <c r="I16" s="54">
         <v>3</v>
       </c>
-      <c r="J12" s="8">
-        <v>7</v>
-      </c>
-      <c r="K12" s="8">
+      <c r="J16" s="54">
+        <v>9</v>
+      </c>
+      <c r="K16" s="54">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="I13" s="8">
-        <v>3</v>
-      </c>
-      <c r="J13" s="8">
-        <v>8</v>
-      </c>
-      <c r="K13" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" s="8">
-        <v>3</v>
-      </c>
-      <c r="J14" s="8">
-        <v>8</v>
-      </c>
-      <c r="K14" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="I15" s="8">
-        <v>3</v>
-      </c>
-      <c r="J15" s="8">
-        <v>9</v>
-      </c>
-      <c r="K15" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
-        <v>14</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="8">
-        <v>3</v>
-      </c>
-      <c r="J16" s="8">
-        <v>9</v>
-      </c>
-      <c r="K16" s="8">
-        <v>6</v>
-      </c>
-    </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B18" s="37"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="19"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="H18" s="18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="H19" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>1</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>114</v>
+      <c r="B20" s="34" t="s">
+        <v>93</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>110</v>
+        <v>81</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="58">
+        <v>32778</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="G20" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>2</v>
       </c>
-      <c r="B21" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>111</v>
+      <c r="B21" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="58">
+        <v>34239</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="12">
+      <c r="A22" s="11">
         <v>3</v>
       </c>
-      <c r="B22" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>117</v>
+      <c r="B22" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="58">
+        <v>36305</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="13">
+      <c r="A23" s="12">
         <v>4</v>
       </c>
-      <c r="B23" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="30" t="s">
+      <c r="B23" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="59">
+        <v>34411</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="G23" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G3" r:id="rId1" display="mailto:anjasmalisi@gmail.com" xr:uid="{D9F97AE9-2F69-42EA-8696-FF28E135EDFE}"/>
+    <hyperlink ref="G4" r:id="rId2" display="mailto:kalll0808@gmail.com" xr:uid="{F67A5788-D7AC-4C72-A669-332FD84E6190}"/>
+    <hyperlink ref="G5" r:id="rId3" display="mailto:anangm123@gmail.com" xr:uid="{52AB6CB8-CE07-40E4-A9AE-25AAA165F6CD}"/>
+    <hyperlink ref="G6" r:id="rId4" display="mailto:asep0201@gmail.com" xr:uid="{C555D68F-F56F-4545-8601-A6E03333AE85}"/>
+    <hyperlink ref="G9" r:id="rId5" display="mailto:friyfauziah@gmail.com" xr:uid="{11653488-BB8C-402E-A3F0-ABD40CC3FC6C}"/>
+    <hyperlink ref="G10" r:id="rId6" display="mailto:jhnptr078@gmail.com" xr:uid="{CCA9174A-6939-4712-A226-21C427EE5F4B}"/>
+    <hyperlink ref="G11" r:id="rId7" display="mailto:barzzcloren@gmail.com" xr:uid="{7DE95C43-529E-405D-A0F8-CD1CF9A5A170}"/>
+    <hyperlink ref="G12" r:id="rId8" display="mailto:rahmatdani123new@gmail.com" xr:uid="{7D508B70-7EC0-43F4-97E6-460E98D012FE}"/>
+    <hyperlink ref="G13" r:id="rId9" display="mailto:ecaraesha694@gmail.com" xr:uid="{8FDE682B-21C9-4A17-AC37-9D45A4F7DDE3}"/>
+    <hyperlink ref="G14" r:id="rId10" display="mailto:eris18789@gmail.com" xr:uid="{158C732A-376F-4CB0-8903-48790E09260F}"/>
+    <hyperlink ref="G15" r:id="rId11" display="mailto:agengmuholapi@gmail.com" xr:uid="{88C7832F-9876-4352-9170-425F026D5C2A}"/>
+    <hyperlink ref="G16" r:id="rId12" display="mailto:atikahdenur@gmail.com" xr:uid="{DA1B6C20-0E61-474B-96B2-18BFB626FB2B}"/>
+    <hyperlink ref="G20" r:id="rId13" xr:uid="{4E0CA5F3-9309-44AC-A597-4688036C2546}"/>
+    <hyperlink ref="G21" r:id="rId14" xr:uid="{E5D95008-4B64-4804-A40F-46F4005B9969}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>